<commit_message>
Register & log in TCs 03.03
</commit_message>
<xml_diff>
--- a/testdata/test_archive.xlsx
+++ b/testdata/test_archive.xlsx
@@ -20,6 +20,8 @@
     <sheet name="Two last names" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Two first names" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="Existing username" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Different passwords" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Database verification" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1897,7 +1899,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2108,7 +2110,7 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>45717.90519327052</v>
+        <v>45717.90519327547</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2158,6 +2160,1156 @@
       <c r="L4" t="inlineStr">
         <is>
           <t>(V7AHwm%se</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>45719.83218118056</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Igor</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Moryc</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ulica Kasztanowa 35/17</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Ostrów Mazowiecka</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Lubelskie</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>39-194</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>519 130 953</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>99072765780</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>igor_mor</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>$+40KsFM+$</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>45719.84338392361</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Maksymilian</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Żywica</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ulica Krasickiego 534</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Piekary Śląskie</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Podlaskie</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>65-632</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>730 582 732</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>16252768012</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>maksymilian</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>(V7AHwm%se</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>45719.84787918982</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Jakub</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pezda</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>plac Mazowiecka 88</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Kluczbork</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Podkarpackie</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>35-903</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>+48 607 956 141</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>95012292275</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>jakub_pe</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>(V15YXkv7E</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>45719.85717928241</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Jakub</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Pezda</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>plac Mazowiecka 88</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Kluczbork</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Podkarpackie</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>35-903</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>+48 607 956 141</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>95012292275</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>jakub_pe</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>(V15YXkv7E</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Date &amp; time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>firstname</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>lastname</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>streetaddress</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>city</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>state</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>postcode</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>phonenumber</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>ssn</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>password</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>45719.84791469907</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Liwia</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Gzyl</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>al. Mazowiecka 61</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Jastrzębie-Zdrój</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>64-798</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>+48 791 593 589</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>19322164246</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>kzywica</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>4GtN*hv0*Y</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>45719.85720462963</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Maksymilian</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Komisarczyk</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>pl. Kolonia 39/34</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Chojnice</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Opolskie</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>70-122</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>+48 503 361 238</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>75102465543</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>marcinbosek</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>kkRuqNtR#9</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Date &amp; time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>firstname</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>lastname</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>streetaddress</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>city</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>state</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>postcode</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>phonenumber</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>ssn</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>password</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>45719.85760917824</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Tymon</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Sabała</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ulica Bydgoska 550</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Kielce</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Zachodniopomorskie</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>02-009</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>+48 733 510 413</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>12292369578</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>arkadiuszrzezniczek</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>QWF6fsjk&amp;3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>45719.85809120371</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Maciej</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Kurcz</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>al. Broniewskiego 63</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Kluczbork</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Wielkopolskie</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>32-906</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>507 015 051</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>78112951369</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>oskarjonczyk</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>AV!g5FAxc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>45719.86011217593</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Radosław</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Wydmuch</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>aleja Dworska 426</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Swarzędz</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Mazowieckie</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>39-103</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>+48 789 740 913</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>24210649228</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>marikaklaja</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>%^3YXwHj4D</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>45719.86066746528</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Bianka</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sapała</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>aleja Waryńskiego 548</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Świętochłowice</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Śląskie</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>58-775</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>+48 22 508 09 00</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>81112408915</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>upeksa</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>b9#MbuFX(V</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>45719.86157180556</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Jędrzej</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Mrózek</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ul. Reymonta 19/56</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Pruszcz Gdański</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>23-434</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>+48 32 039 64 36</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>99071546751</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nkuban</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>)2DWkMhFV8</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>45719.86267232639</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Kamila</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Wawrzynowicz</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>pl. Południowa 212</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Świętochłowice</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Lubelskie</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>05-777</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>794 362 300</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>86122582770</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>karina06</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>@lISCIkwx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>45719.86440782408</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Borys</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Siara</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ulica Długa 09</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Krotoszyn</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Kujawsko - pomorskie</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>41-880</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>+48 720 718 425</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>06242147242</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>ada14</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>+2TCa3H0P3</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>45719.86669033565</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Tomasz</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Cieciura</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>al. Bursztynowa 73</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Chorzów</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Kujawsko - pomorskie</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>38-993</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>734 451 473</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>00251209133</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>sebastian82</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>w_2L+aIr4A</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>45719.89587921296</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Potęga</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>pl. Brzechwy 87</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Piekary Śląskie</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Dolnośląskie</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>65-377</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>603 449 853</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>17271641395</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>ingaczura</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>E8^2+CNmnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>New customer registration</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>45719.89811395122</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Sonia</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Sporysz</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>aleja Odrzańska 81/28</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Gniezno</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Lubuskie</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>75-530</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>607 196 066</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>98040288113</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>bielasstanislaw</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>((a2UYh_f^</t>
         </is>
       </c>
     </row>

</xml_diff>